<commit_message>
Foreign Key Using email changing
</commit_message>
<xml_diff>
--- a/public/template/Template DSRT.xlsx
+++ b/public/template/Template DSRT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irfansbom\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sites\siemas\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AD7FE4-CEE0-43BC-80EC-FCE0057D1D9B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72FAC1A-D75D-43CE-832B-46BF2401B832}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{36FFCFD2-28EE-4F14-83D1-E1487A1EB149}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>KD KAB</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>Beni</t>
+  </si>
+  <si>
+    <t>pencacah</t>
+  </si>
+  <si>
+    <t>pcl01@bpssumsel.com</t>
   </si>
 </sst>
 </file>
@@ -86,7 +92,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -95,6 +101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +419,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD1048576"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +446,9 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -457,6 +466,9 @@
       <c r="E2">
         <v>3</v>
       </c>
+      <c r="F2" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -473,6 +485,9 @@
       </c>
       <c r="E3">
         <v>5</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>